<commit_message>
compute portfolio_complexity and plot the graph over time
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/daywise_full_portfolio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Proportion</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -495,6 +500,9 @@
       <c r="G2" t="n">
         <v>395.9999847412109</v>
       </c>
+      <c r="H2" t="n">
+        <v>0.2024602832988485</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -522,6 +530,9 @@
       <c r="G3" t="n">
         <v>1559.939117431641</v>
       </c>
+      <c r="H3" t="n">
+        <v>0.7975397167011515</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -549,6 +560,9 @@
       <c r="G4" t="n">
         <v>487.3875045776367</v>
       </c>
+      <c r="H4" t="n">
+        <v>0.2320683912910165</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -576,6 +590,9 @@
       <c r="G5" t="n">
         <v>1612.80158996582</v>
       </c>
+      <c r="H5" t="n">
+        <v>0.7679316087089835</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -603,6 +620,9 @@
       <c r="G6" t="n">
         <v>795.5000305175781</v>
       </c>
+      <c r="H6" t="n">
+        <v>0.327064859280383</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -630,6 +650,9 @@
       <c r="G7" t="n">
         <v>1636.739349365234</v>
       </c>
+      <c r="H7" t="n">
+        <v>0.672935140719617</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -657,6 +680,9 @@
       <c r="G8" t="n">
         <v>830</v>
       </c>
+      <c r="H8" t="n">
+        <v>0.1998387472810739</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -684,6 +710,9 @@
       <c r="G9" t="n">
         <v>3323.348693847656</v>
       </c>
+      <c r="H9" t="n">
+        <v>0.8001612527189261</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -711,6 +740,9 @@
       <c r="G10" t="n">
         <v>1708.999938964844</v>
       </c>
+      <c r="H10" t="n">
+        <v>0.29448549770074</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -738,6 +770,9 @@
       <c r="G11" t="n">
         <v>4094.341659545898</v>
       </c>
+      <c r="H11" t="n">
+        <v>0.70551450229926</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -765,6 +800,9 @@
       <c r="G12" t="n">
         <v>1738.000030517578</v>
       </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -792,6 +830,9 @@
       <c r="G13" t="n">
         <v>1923.000030517578</v>
       </c>
+      <c r="H13" t="n">
+        <v>0.285609114310247</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -819,6 +860,9 @@
       <c r="G14" t="n">
         <v>4809.978485107422</v>
       </c>
+      <c r="H14" t="n">
+        <v>0.714390885689753</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -846,6 +890,9 @@
       <c r="G15" t="n">
         <v>1990</v>
       </c>
+      <c r="H15" t="n">
+        <v>0.1899748530660442</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -873,6 +920,9 @@
       <c r="G16" t="n">
         <v>5408.420562744141</v>
       </c>
+      <c r="H16" t="n">
+        <v>0.5163135184556231</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -900,6 +950,9 @@
       <c r="G17" t="n">
         <v>3076.650047302246</v>
       </c>
+      <c r="H17" t="n">
+        <v>0.2937116284783327</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -927,6 +980,9 @@
       <c r="G18" t="n">
         <v>2529.999923706055</v>
       </c>
+      <c r="H18" t="n">
+        <v>0.1965699741749239</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -954,6 +1010,9 @@
       <c r="G19" t="n">
         <v>6056.234436035156</v>
       </c>
+      <c r="H19" t="n">
+        <v>0.470543036596166</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -981,6 +1040,9 @@
       <c r="G20" t="n">
         <v>3082.699966430664</v>
       </c>
+      <c r="H20" t="n">
+        <v>0.2395123601042123</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1008,6 +1070,9 @@
       <c r="G21" t="n">
         <v>1201.800048828125</v>
       </c>
+      <c r="H21" t="n">
+        <v>0.09337462912469786</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1035,6 +1100,9 @@
       <c r="G22" t="n">
         <v>3325.499954223633</v>
       </c>
+      <c r="H22" t="n">
+        <v>0.2345299855249004</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1062,6 +1130,9 @@
       <c r="G23" t="n">
         <v>5837.803344726562</v>
       </c>
+      <c r="H23" t="n">
+        <v>0.4117095031671932</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1089,6 +1160,9 @@
       <c r="G24" t="n">
         <v>3769.020080566406</v>
       </c>
+      <c r="H24" t="n">
+        <v>0.2658091225698614</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1116,6 +1190,9 @@
       <c r="G25" t="n">
         <v>1247.099975585938</v>
       </c>
+      <c r="H25" t="n">
+        <v>0.08795138873804499</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1143,6 +1220,9 @@
       <c r="G26" t="n">
         <v>3185.999908447266</v>
       </c>
+      <c r="H26" t="n">
+        <v>0.2202929848295488</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1170,6 +1250,9 @@
       <c r="G27" t="n">
         <v>5532.597198486328</v>
       </c>
+      <c r="H27" t="n">
+        <v>0.3825462604323004</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1197,6 +1280,9 @@
       <c r="G28" t="n">
         <v>4490.36018371582</v>
       </c>
+      <c r="H28" t="n">
+        <v>0.3104817565147436</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1224,6 +1310,9 @@
       <c r="G29" t="n">
         <v>1253.599975585938</v>
       </c>
+      <c r="H29" t="n">
+        <v>0.08667899822340711</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1251,6 +1340,9 @@
       <c r="G30" t="n">
         <v>3596.25</v>
       </c>
+      <c r="H30" t="n">
+        <v>0.2107788414767302</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1278,6 +1370,9 @@
       <c r="G31" t="n">
         <v>5849.772033691406</v>
       </c>
+      <c r="H31" t="n">
+        <v>0.3428594152699202</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1305,6 +1400,9 @@
       <c r="G32" t="n">
         <v>6373.600006103516</v>
       </c>
+      <c r="H32" t="n">
+        <v>0.3735613556684267</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1332,6 +1430,9 @@
       <c r="G33" t="n">
         <v>1242.099975585938</v>
       </c>
+      <c r="H33" t="n">
+        <v>0.07280038758492284</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1359,6 +1460,9 @@
       <c r="G34" t="n">
         <v>3437.175037384033</v>
       </c>
+      <c r="H34" t="n">
+        <v>0.3066465430776691</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1386,6 +1490,9 @@
       <c r="G35" t="n">
         <v>6492.7099609375</v>
       </c>
+      <c r="H35" t="n">
+        <v>0.5792451775289043</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1413,6 +1520,9 @@
       <c r="G36" t="n">
         <v>1279.030004882813</v>
       </c>
+      <c r="H36" t="n">
+        <v>0.1141082793934266</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1440,6 +1550,9 @@
       <c r="G37" t="n">
         <v>3318.000106811523</v>
       </c>
+      <c r="H37" t="n">
+        <v>0.2757012999576651</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1467,6 +1580,9 @@
       <c r="G38" t="n">
         <v>6665.799713134766</v>
       </c>
+      <c r="H38" t="n">
+        <v>0.5538787182061652</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1494,6 +1610,9 @@
       <c r="G39" t="n">
         <v>1365</v>
       </c>
+      <c r="H39" t="n">
+        <v>0.1134214172174498</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1521,6 +1640,9 @@
       <c r="G40" t="n">
         <v>685.9642791748047</v>
       </c>
+      <c r="H40" t="n">
+        <v>0.05699856461871995</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1548,6 +1670,9 @@
       <c r="G41" t="n">
         <v>3722.000122070312</v>
       </c>
+      <c r="H41" t="n">
+        <v>0.267700449473472</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1575,6 +1700,9 @@
       <c r="G42" t="n">
         <v>6626.899719238281</v>
       </c>
+      <c r="H42" t="n">
+        <v>0.4766319116800394</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1602,6 +1730,9 @@
       <c r="G43" t="n">
         <v>1327</v>
       </c>
+      <c r="H43" t="n">
+        <v>0.09544290295554872</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1629,6 +1760,9 @@
       <c r="G44" t="n">
         <v>2227.700729370117</v>
       </c>
+      <c r="H44" t="n">
+        <v>0.1602247358909399</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1656,6 +1790,9 @@
       <c r="G45" t="n">
         <v>3473.999938964844</v>
       </c>
+      <c r="H45" t="n">
+        <v>0.1958556412857424</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1683,6 +1820,9 @@
       <c r="G46" t="n">
         <v>10244.2497253418</v>
       </c>
+      <c r="H46" t="n">
+        <v>0.5775458073398694</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1710,6 +1850,9 @@
       <c r="G47" t="n">
         <v>1293.400024414062</v>
       </c>
+      <c r="H47" t="n">
+        <v>0.07291873795947541</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1737,6 +1880,9 @@
       <c r="G48" t="n">
         <v>2725.903930664062</v>
       </c>
+      <c r="H48" t="n">
+        <v>0.1536798134149128</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1764,6 +1910,9 @@
       <c r="G49" t="n">
         <v>3017.999877929688</v>
       </c>
+      <c r="H49" t="n">
+        <v>0.1606830912658308</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1791,6 +1940,9 @@
       <c r="G50" t="n">
         <v>10710.68027496338</v>
       </c>
+      <c r="H50" t="n">
+        <v>0.5702535738078549</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1818,6 +1970,9 @@
       <c r="G51" t="n">
         <v>1147.300048828125</v>
       </c>
+      <c r="H51" t="n">
+        <v>0.06108407087862602</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1845,6 +2000,9 @@
       <c r="G52" t="n">
         <v>3906.331329345703</v>
       </c>
+      <c r="H52" t="n">
+        <v>0.2079792640476884</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1872,6 +2030,9 @@
       <c r="G53" t="n">
         <v>1831.999969482422</v>
       </c>
+      <c r="H53" t="n">
+        <v>0.1182621707680098</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1899,6 +2060,9 @@
       <c r="G54" t="n">
         <v>10534.99984741211</v>
       </c>
+      <c r="H54" t="n">
+        <v>0.6800720369813099</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1926,6 +2090,9 @@
       <c r="G55" t="n">
         <v>821.5</v>
       </c>
+      <c r="H55" t="n">
+        <v>0.05303077232766965</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1952,6 +2119,9 @@
       </c>
       <c r="G56" t="n">
         <v>2302.505950927734</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.1486350199230106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>